<commit_message>
Agregar NodePort a SonarQube
</commit_message>
<xml_diff>
--- a/estimacion/Requisitos Infraestructura DevOps.xlsx
+++ b/estimacion/Requisitos Infraestructura DevOps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imendozah/Documents/trabajo/grupo-accelera/atos/integra-cam/estimacion-plataform-dev-devops/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imendozah/Documents/GitHub/devops-doc-itc/estimacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A344241-29C6-F04B-B1F1-90B85A711767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2406BC9D-604C-7D41-9CC6-94FF7796F58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{E63569D2-4900-4C19-90F0-9A15FCC0B5C2}"/>
+    <workbookView xWindow="29720" yWindow="1500" windowWidth="28800" windowHeight="16120" xr2:uid="{E63569D2-4900-4C19-90F0-9A15FCC0B5C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Software" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="79">
   <si>
     <t>Tecnología</t>
   </si>
@@ -264,6 +264,15 @@
   </si>
   <si>
     <t>t3a.medium</t>
+  </si>
+  <si>
+    <t>NodePort: 30001</t>
+  </si>
+  <si>
+    <t>NodePort: 3xxxx</t>
+  </si>
+  <si>
+    <t>9.5.0</t>
   </si>
 </sst>
 </file>
@@ -508,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -607,6 +616,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -921,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7C5B99-D1D0-4E3F-82AC-30B3273A27E8}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="158" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="158" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -933,9 +943,10 @@
     <col min="2" max="2" width="32.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
         <v>66</v>
       </c>
@@ -944,7 +955,7 @@
       <c r="D1" s="30"/>
       <c r="E1" s="30"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>61</v>
       </c>
@@ -961,7 +972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -978,7 +989,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -995,7 +1006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1012,7 +1023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
         <v>63</v>
       </c>
@@ -1021,7 +1032,7 @@
       <c r="D7" s="30"/>
       <c r="E7" s="30"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>61</v>
       </c>
@@ -1038,7 +1049,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -1054,8 +1065,11 @@
       <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -1072,7 +1086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -1082,14 +1096,17 @@
       <c r="C11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="12">
-        <v>8.1999999999999993</v>
+      <c r="D11" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>4</v>
       </c>
@@ -1106,7 +1123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>5</v>
       </c>
@@ -1123,7 +1140,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>6</v>
       </c>
@@ -1140,7 +1157,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>7</v>
       </c>
@@ -1157,7 +1174,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="25"/>
       <c r="B16" s="25"/>
       <c r="C16" s="25"/>
@@ -1351,7 +1368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4634B6F5-F15A-CC48-9949-2532B69B3B0F}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="125" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update Requisitos Infraestructura DevOps.xlsx
</commit_message>
<xml_diff>
--- a/estimacion/Requisitos Infraestructura DevOps.xlsx
+++ b/estimacion/Requisitos Infraestructura DevOps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imendozah/Documents/GitHub/devops-doc-itc/estimacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2406BC9D-604C-7D41-9CC6-94FF7796F58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA521EA-B36B-3D4E-8B84-E0403E982E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29720" yWindow="1500" windowWidth="28800" windowHeight="16120" xr2:uid="{E63569D2-4900-4C19-90F0-9A15FCC0B5C2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{E63569D2-4900-4C19-90F0-9A15FCC0B5C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Software" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="84">
   <si>
     <t>Tecnología</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Base de Datos</t>
   </si>
   <si>
-    <t>Jenkins</t>
-  </si>
-  <si>
     <t>Automatización CI</t>
   </si>
   <si>
@@ -94,15 +91,9 @@
     <t>Apache Kafka Broker</t>
   </si>
   <si>
-    <t>JFrog Artifactory</t>
-  </si>
-  <si>
     <t>Gestor de contenedores</t>
   </si>
   <si>
-    <t>JFrog Container Registry</t>
-  </si>
-  <si>
     <t>Terraform</t>
   </si>
   <si>
@@ -112,9 +103,6 @@
     <t>PostgreSQL</t>
   </si>
   <si>
-    <t>SonarQube</t>
-  </si>
-  <si>
     <t>Calidad de software</t>
   </si>
   <si>
@@ -203,9 +191,6 @@
   </si>
   <si>
     <t>CentOs</t>
-  </si>
-  <si>
-    <t>1.9+</t>
   </si>
   <si>
     <t>6.+</t>
@@ -266,13 +251,43 @@
     <t>t3a.medium</t>
   </si>
   <si>
-    <t>NodePort: 30001</t>
-  </si>
-  <si>
-    <t>NodePort: 3xxxx</t>
-  </si>
-  <si>
     <t>9.5.0</t>
+  </si>
+  <si>
+    <t>Gestión de seguridad</t>
+  </si>
+  <si>
+    <t>18.0.2-debian-11-r28</t>
+  </si>
+  <si>
+    <t>Keycloak (kubernetes)</t>
+  </si>
+  <si>
+    <t>OpenLDAP (kubernetes)</t>
+  </si>
+  <si>
+    <t>2.368-jdk17</t>
+  </si>
+  <si>
+    <t>Jenkins (Kubernetes)</t>
+  </si>
+  <si>
+    <t>2.4.50</t>
+  </si>
+  <si>
+    <t>Gestor de LDAP</t>
+  </si>
+  <si>
+    <t>Gestor de acceso e identidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SonarQube  (Kubernetes) </t>
+  </si>
+  <si>
+    <t>JFrog Container Registry  (Kubernetes)</t>
+  </si>
+  <si>
+    <t>JFrog Artifactory  (Kubernetes)</t>
   </si>
 </sst>
 </file>
@@ -517,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -592,6 +607,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -616,7 +635,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -931,33 +949,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7C5B99-D1D0-4E3F-82AC-30B3273A27E8}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="158" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="158" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="A1" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -977,16 +995,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D3" s="11">
         <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -994,16 +1012,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1011,30 +1029,30 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
+      <c r="A7" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>0</v>
@@ -1054,36 +1072,34 @@
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="38" t="s">
-        <v>77</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F9" s="31"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1091,36 +1107,34 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="38" t="s">
-        <v>76</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F11" s="31"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>4</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1128,16 +1142,16 @@
         <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1145,16 +1159,16 @@
         <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1162,16 +1176,16 @@
         <v>7</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1182,17 +1196,17 @@
       <c r="E16" s="25"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
+      <c r="A17" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>0</v>
@@ -1212,16 +1226,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1229,16 +1243,16 @@
         <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1249,27 +1263,27 @@
         <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
+      <c r="A23" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>0</v>
@@ -1289,16 +1303,16 @@
         <v>1</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D25" s="11">
         <v>1.24</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1306,16 +1320,16 @@
         <v>2</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1323,16 +1337,16 @@
         <v>3</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>17</v>
-      </c>
       <c r="E27" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1340,24 +1354,85 @@
         <v>4</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>1</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>2</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="A23:E23"/>
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A31:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1382,32 +1457,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="A1" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="32"/>
+        <v>29</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B3" s="6">
         <v>2</v>
@@ -1419,12 +1494,12 @@
         <v>64</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B4" s="6">
         <v>2</v>
@@ -1436,12 +1511,12 @@
         <v>64</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B5" s="6">
         <v>2</v>
@@ -1453,12 +1528,12 @@
         <v>64</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6" s="6">
         <v>2</v>
@@ -1470,15 +1545,15 @@
         <v>10</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B7" s="8">
         <v>2</v>
@@ -1490,12 +1565,12 @@
         <v>64</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B8" s="20">
         <f>SUM(B3:B7)</f>
@@ -1511,32 +1586,32 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="37"/>
+      <c r="A10" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="39"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B12" s="6">
         <v>4</v>
@@ -1548,12 +1623,12 @@
         <v>64</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B13" s="6">
         <v>8</v>
@@ -1565,12 +1640,12 @@
         <v>128</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B14" s="6">
         <v>4</v>
@@ -1582,12 +1657,12 @@
         <v>64</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B15" s="18">
         <v>2</v>
@@ -1599,12 +1674,12 @@
         <v>64</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="28" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B16" s="8">
         <v>2</v>
@@ -1616,12 +1691,12 @@
         <v>512</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B17" s="29">
         <f>SUM(B12:B16)</f>
@@ -1637,32 +1712,32 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
+      <c r="A19" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="39"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="32"/>
+        <v>29</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="34"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B21" s="6">
         <v>4</v>
@@ -1674,12 +1749,12 @@
         <v>64</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B22" s="6">
         <v>4</v>
@@ -1691,12 +1766,12 @@
         <v>64</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B23" s="6">
         <v>8</v>
@@ -1708,12 +1783,12 @@
         <v>128</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B24" s="6">
         <v>4</v>
@@ -1725,12 +1800,12 @@
         <v>64</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B25" s="6">
         <v>4</v>
@@ -1742,12 +1817,12 @@
         <v>64</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B26" s="6">
         <v>4</v>
@@ -1759,12 +1834,12 @@
         <v>64</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B27" s="18">
         <v>4</v>
@@ -1776,12 +1851,12 @@
         <v>64</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B28" s="8">
         <v>2</v>
@@ -1793,12 +1868,12 @@
         <v>512</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="23" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B29" s="20">
         <f>SUM(B21:B28)</f>
@@ -1814,32 +1889,32 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
+      <c r="A31" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="32"/>
+        <v>29</v>
+      </c>
+      <c r="D32" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="34"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B33" s="6">
         <v>2</v>
@@ -1851,12 +1926,12 @@
         <v>64</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.2">
       <c r="A34" s="27" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B34" s="6">
         <v>4</v>
@@ -1868,12 +1943,12 @@
         <v>64</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B35" s="6">
         <v>2</v>
@@ -1885,12 +1960,12 @@
         <v>32</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="23" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B36" s="20">
         <f>SUM(B33:B35)</f>

</xml_diff>